<commit_message>
recup du form et injection id nom prenom ok
</commit_message>
<xml_diff>
--- a/creatXl.xlsx
+++ b/creatXl.xlsx
@@ -15,7 +15,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="0"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
+  <si>
+    <t>Cherief</t>
+  </si>
+  <si>
+    <t>Saufiane</t>
+  </si>
+  <si>
+    <t>toto</t>
+  </si>
+  <si>
+    <t>tata</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -352,14 +365,37 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
insert_passage ok create_escel ok
</commit_message>
<xml_diff>
--- a/creatXl.xlsx
+++ b/creatXl.xlsx
@@ -15,7 +15,61 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="28">
+  <si>
+    <t>id_participants</t>
+  </si>
+  <si>
+    <t>Nom</t>
+  </si>
+  <si>
+    <t>Prenom</t>
+  </si>
+  <si>
+    <t>id_epreuve</t>
+  </si>
+  <si>
+    <t>Epreuve</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Temps 1</t>
+  </si>
+  <si>
+    <t>Temps 2</t>
+  </si>
+  <si>
+    <t>Meilleur Temps</t>
+  </si>
+  <si>
+    <t>id_categorie</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Génique</t>
+  </si>
+  <si>
+    <t>Yoann</t>
+  </si>
+  <si>
+    <t>La Descente des Alpes - M1</t>
+  </si>
+  <si>
+    <t>2021-02-27</t>
+  </si>
+  <si>
+    <t>M1</t>
+  </si>
+  <si>
+    <t>Mairot</t>
+  </si>
+  <si>
+    <t>Jean-christophe</t>
+  </si>
   <si>
     <t>Cherief</t>
   </si>
@@ -23,10 +77,28 @@
     <t>Saufiane</t>
   </si>
   <si>
+    <t>Rameau</t>
+  </si>
+  <si>
+    <t>Célia</t>
+  </si>
+  <si>
+    <t>Ligourel</t>
+  </si>
+  <si>
+    <t>Teedji</t>
+  </si>
+  <si>
     <t>toto</t>
   </si>
   <si>
     <t>tata</t>
+  </si>
+  <si>
+    <t>choula</t>
+  </si>
+  <si>
+    <t>poula</t>
   </si>
 </sst>
 </file>
@@ -365,7 +437,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -373,26 +445,221 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1">
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correction de bug et redirection
</commit_message>
<xml_diff>
--- a/creatXl.xlsx
+++ b/creatXl.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
   <si>
     <t>id_participants</t>
   </si>
@@ -48,6 +48,63 @@
   </si>
   <si>
     <t>Type</t>
+  </si>
+  <si>
+    <t>Génique</t>
+  </si>
+  <si>
+    <t>Yoann</t>
+  </si>
+  <si>
+    <t>La Descente des Alpes - M1</t>
+  </si>
+  <si>
+    <t>2021-02-27</t>
+  </si>
+  <si>
+    <t>M1</t>
+  </si>
+  <si>
+    <t>Mairot</t>
+  </si>
+  <si>
+    <t>Jean-christophe</t>
+  </si>
+  <si>
+    <t>Cherief</t>
+  </si>
+  <si>
+    <t>Saufiane</t>
+  </si>
+  <si>
+    <t>Rameau</t>
+  </si>
+  <si>
+    <t>Célia</t>
+  </si>
+  <si>
+    <t>Ligourel</t>
+  </si>
+  <si>
+    <t>Teedji</t>
+  </si>
+  <si>
+    <t>toto</t>
+  </si>
+  <si>
+    <t>tata</t>
+  </si>
+  <si>
+    <t>choula</t>
+  </si>
+  <si>
+    <t>poula</t>
+  </si>
+  <si>
+    <t>mairot</t>
+  </si>
+  <si>
+    <t>tutu</t>
   </si>
 </sst>
 </file>
@@ -386,7 +443,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -427,6 +484,214 @@
       </c>
       <c r="K1" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>